<commit_message>
fixed session and task methods
Added Get Session Log call
</commit_message>
<xml_diff>
--- a/ServiceTestMatrix.xlsx
+++ b/ServiceTestMatrix.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="31">
   <si>
     <t>Endpoint</t>
   </si>
@@ -96,7 +96,19 @@
     <t>{"finish":{"sessionId":1376968156,"taskId":1}}</t>
   </si>
   <si>
-    <t>Broken</t>
+    <t>log</t>
+  </si>
+  <si>
+    <t>log[sessionId]=1377057169&amp;log[conditionId]=3&amp;log[taskId]=0</t>
+  </si>
+  <si>
+    <t>config[sessionId]=1377058693&amp;config[taskId]=1</t>
+  </si>
+  <si>
+    <t>open</t>
+  </si>
+  <si>
+    <t>transition</t>
   </si>
 </sst>
 </file>
@@ -126,12 +138,18 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -146,20 +164,26 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFFFF99"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -455,14 +479,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I15"/>
+  <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7:I8"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="5" max="5" width="30.5703125" customWidth="1"/>
     <col min="6" max="7" width="43.5703125" customWidth="1"/>
     <col min="8" max="9" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
@@ -517,67 +542,68 @@
         <f>CONCATENATE("http://localhost/rbwatson/",A2,".php", IF(D2&lt;&gt;"","?",""),D2)</f>
         <v>http://localhost/rbwatson/study.php?config[studyId]=1234&amp;config[conditionId]=4&amp;config[taskId]=1</v>
       </c>
-      <c r="H2" s="4">
+      <c r="H2" s="3">
         <v>41504</v>
       </c>
-      <c r="I2" s="4">
+      <c r="I2" s="3">
         <v>41504</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D3" s="3"/>
-      <c r="E3" t="s">
+      <c r="D3" s="5"/>
+      <c r="E3" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="F3" t="str">
-        <f t="shared" ref="F3:F15" si="0">CONCATENATE("http://wlux.uw.edu/rbwatson/",A3,".php", IF(D3&lt;&gt;"","?",""),D3)</f>
+      <c r="F3" s="4" t="str">
+        <f t="shared" ref="F3:F16" si="0">CONCATENATE("http://wlux.uw.edu/rbwatson/",A3,".php", IF(D3&lt;&gt;"","?",""),D3)</f>
         <v>http://wlux.uw.edu/rbwatson/study.php</v>
       </c>
-      <c r="G3" t="str">
+      <c r="G3" s="4" t="str">
         <f>CONCATENATE("http://localhost/rbwatson/",A3,".php", IF(D3&lt;&gt;"","?",""),D3)</f>
         <v>http://localhost/rbwatson/study.php</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I3" s="4" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E4" t="s">
+      <c r="D4" s="4"/>
+      <c r="E4" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="F4" t="str">
+      <c r="F4" s="4" t="str">
         <f t="shared" si="0"/>
         <v>http://wlux.uw.edu/rbwatson/study.php</v>
       </c>
-      <c r="G4" t="str">
-        <f t="shared" ref="G4:G15" si="1">CONCATENATE("http://localhost/rbwatson/",A4,".php", IF(D4&lt;&gt;"","?",""),D4)</f>
+      <c r="G4" s="4" t="str">
+        <f t="shared" ref="G4:G16" si="1">CONCATENATE("http://localhost/rbwatson/",A4,".php", IF(D4&lt;&gt;"","?",""),D4)</f>
         <v>http://localhost/rbwatson/study.php</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="I4" t="s">
+      <c r="I4" s="4" t="s">
         <v>13</v>
       </c>
     </row>
@@ -602,10 +628,10 @@
         <f t="shared" si="1"/>
         <v>http://localhost/rbwatson/session.php</v>
       </c>
-      <c r="H5" s="4">
+      <c r="H5" s="3">
         <v>41504</v>
       </c>
-      <c r="I5" s="4">
+      <c r="I5" s="3">
         <v>41504</v>
       </c>
     </row>
@@ -630,10 +656,10 @@
         <f t="shared" si="1"/>
         <v>http://localhost/rbwatson/task.php</v>
       </c>
-      <c r="H6" s="4">
+      <c r="H6" s="3">
         <v>41504</v>
       </c>
-      <c r="I6" s="4">
+      <c r="I6" s="3">
         <v>41504</v>
       </c>
     </row>
@@ -658,10 +684,10 @@
         <f t="shared" si="1"/>
         <v>http://localhost/rbwatson/task.php</v>
       </c>
-      <c r="H7" t="s">
-        <v>26</v>
-      </c>
-      <c r="I7" s="4">
+      <c r="H7" s="3">
+        <v>41504</v>
+      </c>
+      <c r="I7" s="3">
         <v>41504</v>
       </c>
     </row>
@@ -686,82 +712,205 @@
         <f t="shared" si="1"/>
         <v>http://localhost/rbwatson/session.php</v>
       </c>
-      <c r="H8" t="s">
+      <c r="H8" s="3">
+        <v>41504</v>
+      </c>
+      <c r="I8" s="3">
+        <v>41504</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" t="s">
         <v>26</v>
       </c>
-      <c r="I8" s="4">
-        <v>41504</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D9" t="s">
+        <v>27</v>
+      </c>
       <c r="F9" t="str">
         <f t="shared" si="0"/>
-        <v>http://wlux.uw.edu/rbwatson/.php</v>
+        <v>http://wlux.uw.edu/rbwatson/session.php?log[sessionId]=1377057169&amp;log[conditionId]=3&amp;log[taskId]=0</v>
       </c>
       <c r="G9" t="str">
         <f t="shared" si="1"/>
-        <v>http://localhost/rbwatson/.php</v>
+        <v>http://localhost/rbwatson/session.php?log[sessionId]=1377057169&amp;log[conditionId]=3&amp;log[taskId]=0</v>
+      </c>
+      <c r="H9" s="3">
+        <v>41506</v>
+      </c>
+      <c r="I9" s="3">
+        <v>41506</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="F10" t="str">
-        <f t="shared" si="0"/>
-        <v>http://wlux.uw.edu/rbwatson/.php</v>
-      </c>
-      <c r="G10" t="str">
-        <f t="shared" si="1"/>
-        <v>http://localhost/rbwatson/.php</v>
-      </c>
+      <c r="A10" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>http://wlux.uw.edu/rbwatson/session.php?config[sessionId]=1377058693&amp;config[taskId]=1</v>
+      </c>
+      <c r="G10" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>http://localhost/rbwatson/session.php?config[sessionId]=1377058693&amp;config[taskId]=1</v>
+      </c>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="F11" t="str">
-        <f t="shared" si="0"/>
-        <v>http://wlux.uw.edu/rbwatson/.php</v>
-      </c>
-      <c r="G11" t="str">
-        <f t="shared" si="1"/>
-        <v>http://localhost/rbwatson/.php</v>
-      </c>
+      <c r="A11" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>http://wlux.uw.edu/rbwatson/task.php?config[sessionId]=1377058693&amp;config[taskId]=1</v>
+      </c>
+      <c r="G11" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>http://localhost/rbwatson/task.php?config[sessionId]=1377058693&amp;config[taskId]=1</v>
+      </c>
+      <c r="H11" s="4"/>
+      <c r="I11" s="4"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="F12" t="str">
-        <f t="shared" si="0"/>
-        <v>http://wlux.uw.edu/rbwatson/.php</v>
-      </c>
-      <c r="G12" t="str">
-        <f t="shared" si="1"/>
-        <v>http://localhost/rbwatson/.php</v>
-      </c>
+      <c r="A12" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>http://wlux.uw.edu/rbwatson/log.php</v>
+      </c>
+      <c r="G12" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>http://localhost/rbwatson/log.php</v>
+      </c>
+      <c r="H12" s="4"/>
+      <c r="I12" s="4"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="F13" t="str">
-        <f t="shared" si="0"/>
-        <v>http://wlux.uw.edu/rbwatson/.php</v>
-      </c>
-      <c r="G13" t="str">
-        <f t="shared" si="1"/>
-        <v>http://localhost/rbwatson/.php</v>
-      </c>
+      <c r="A13" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>http://wlux.uw.edu/rbwatson/log.php</v>
+      </c>
+      <c r="G13" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>http://localhost/rbwatson/log.php</v>
+      </c>
+      <c r="H13" s="4"/>
+      <c r="I13" s="4"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="F14" t="str">
-        <f t="shared" si="0"/>
-        <v>http://wlux.uw.edu/rbwatson/.php</v>
-      </c>
-      <c r="G14" t="str">
-        <f t="shared" si="1"/>
-        <v>http://localhost/rbwatson/.php</v>
-      </c>
+      <c r="A14" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>http://wlux.uw.edu/rbwatson/log.php</v>
+      </c>
+      <c r="G14" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>http://localhost/rbwatson/log.php</v>
+      </c>
+      <c r="H14" s="4"/>
+      <c r="I14" s="4"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="F15" t="str">
-        <f t="shared" si="0"/>
-        <v>http://wlux.uw.edu/rbwatson/.php</v>
-      </c>
-      <c r="G15" t="str">
-        <f t="shared" si="1"/>
-        <v>http://localhost/rbwatson/.php</v>
-      </c>
+      <c r="A15" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>http://wlux.uw.edu/rbwatson/log.php</v>
+      </c>
+      <c r="G15" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>http://localhost/rbwatson/log.php</v>
+      </c>
+      <c r="H15" s="4"/>
+      <c r="I15" s="4"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>http://wlux.uw.edu/rbwatson/log.php</v>
+      </c>
+      <c r="G16" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>http://localhost/rbwatson/log.php</v>
+      </c>
+      <c r="H16" s="4"/>
+      <c r="I16" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Adding support for multi-task studies
</commit_message>
<xml_diff>
--- a/ServiceTestMatrix.xlsx
+++ b/ServiceTestMatrix.xlsx
@@ -1,22 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23613"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="135" windowWidth="15315" windowHeight="11310"/>
+    <workbookView xWindow="1820" yWindow="5400" windowWidth="25480" windowHeight="11220"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="33">
   <si>
     <t>Endpoint</t>
   </si>
@@ -109,13 +114,19 @@
   </si>
   <si>
     <t>transition</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>Not writing the correct session/task config record</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -136,6 +147,22 @@
       <color theme="1"/>
       <name val="Cambria"/>
       <family val="1"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -161,8 +188,64 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -174,7 +257,63 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="57">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -479,20 +618,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I16"/>
+  <dimension ref="A1:J16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" topLeftCell="G2" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="5" max="5" width="30.5703125" customWidth="1"/>
-    <col min="6" max="7" width="43.5703125" customWidth="1"/>
-    <col min="8" max="9" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.5" customWidth="1"/>
+    <col min="6" max="7" width="43.5" customWidth="1"/>
+    <col min="8" max="9" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="44.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="29.25" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -520,8 +660,11 @@
       <c r="I1" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J1" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -549,7 +692,7 @@
         <v>41504</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="15">
       <c r="A3" s="4" t="s">
         <v>11</v>
       </c>
@@ -578,7 +721,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10">
       <c r="A4" s="4" t="s">
         <v>11</v>
       </c>
@@ -607,7 +750,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -635,7 +778,7 @@
         <v>41504</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -662,8 +805,11 @@
       <c r="I6" s="3">
         <v>41504</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
       <c r="A7" t="s">
         <v>21</v>
       </c>
@@ -691,7 +837,7 @@
         <v>41504</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -719,7 +865,7 @@
         <v>41504</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -747,7 +893,7 @@
         <v>41506</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10">
       <c r="A10" s="4" t="s">
         <v>17</v>
       </c>
@@ -772,7 +918,7 @@
       <c r="H10" s="4"/>
       <c r="I10" s="4"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10">
       <c r="A11" s="4" t="s">
         <v>21</v>
       </c>
@@ -797,7 +943,7 @@
       <c r="H11" s="4"/>
       <c r="I11" s="4"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10">
       <c r="A12" s="4" t="s">
         <v>26</v>
       </c>
@@ -820,7 +966,7 @@
       <c r="H12" s="4"/>
       <c r="I12" s="4"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10">
       <c r="A13" s="4" t="s">
         <v>26</v>
       </c>
@@ -843,7 +989,7 @@
       <c r="H13" s="4"/>
       <c r="I13" s="4"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10">
       <c r="A14" s="4" t="s">
         <v>26</v>
       </c>
@@ -866,7 +1012,7 @@
       <c r="H14" s="4"/>
       <c r="I14" s="4"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10">
       <c r="A15" s="4" t="s">
         <v>26</v>
       </c>
@@ -889,7 +1035,7 @@
       <c r="H15" s="4"/>
       <c r="I15" s="4"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10">
       <c r="A16" s="4" t="s">
         <v>26</v>
       </c>
@@ -914,7 +1060,12 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" verticalDpi="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -924,9 +1075,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -936,8 +1092,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added more support for multi-task sessions
task: added get-config and fixed post-start & post-finish
session: fixed get-config and get-log to not require a conditionId
updated test matrix
*Did not upload to WLUX*
</commit_message>
<xml_diff>
--- a/ServiceTestMatrix.xlsx
+++ b/ServiceTestMatrix.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23613"/>
-  <workbookPr autoCompressPictures="0"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="1820" yWindow="5400" windowWidth="25480" windowHeight="11220"/>
+    <workbookView xWindow="1815" yWindow="5400" windowWidth="25485" windowHeight="11220"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="32">
   <si>
     <t>Endpoint</t>
   </si>
@@ -117,9 +117,6 @@
   </si>
   <si>
     <t>Comments</t>
-  </si>
-  <si>
-    <t>Not writing the correct session/task config record</t>
   </si>
 </sst>
 </file>
@@ -247,7 +244,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -256,6 +253,7 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="57">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -620,19 +618,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G2" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="30.5" customWidth="1"/>
-    <col min="6" max="7" width="43.5" customWidth="1"/>
-    <col min="8" max="9" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="44.5" customWidth="1"/>
+    <col min="5" max="5" width="30.42578125" customWidth="1"/>
+    <col min="6" max="7" width="43.42578125" customWidth="1"/>
+    <col min="8" max="9" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="44.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="29.25" customHeight="1">
+    <row r="1" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -664,7 +662,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -689,10 +687,10 @@
         <v>41504</v>
       </c>
       <c r="I2" s="3">
-        <v>41504</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="15">
+        <v>41507</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>11</v>
       </c>
@@ -721,7 +719,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>11</v>
       </c>
@@ -750,7 +748,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -775,10 +773,10 @@
         <v>41504</v>
       </c>
       <c r="I5" s="3">
-        <v>41504</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10">
+        <v>41507</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -803,13 +801,10 @@
         <v>41504</v>
       </c>
       <c r="I6" s="3">
-        <v>41504</v>
-      </c>
-      <c r="J6" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10">
+        <v>41507</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>21</v>
       </c>
@@ -834,10 +829,10 @@
         <v>41504</v>
       </c>
       <c r="I7" s="3">
-        <v>41504</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10">
+        <v>41507</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -862,10 +857,10 @@
         <v>41504</v>
       </c>
       <c r="I8" s="3">
-        <v>41504</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10">
+        <v>41507</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -890,60 +885,66 @@
         <v>41506</v>
       </c>
       <c r="I9" s="3">
-        <v>41506</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10">
-      <c r="A10" s="4" t="s">
+        <v>41507</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="D10" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4" t="str">
+      <c r="F10" s="6" t="str">
         <f t="shared" si="0"/>
         <v>http://wlux.uw.edu/rbwatson/session.php?config[sessionId]=1377058693&amp;config[taskId]=1</v>
       </c>
-      <c r="G10" s="4" t="str">
+      <c r="G10" s="6" t="str">
         <f t="shared" si="1"/>
         <v>http://localhost/rbwatson/session.php?config[sessionId]=1377058693&amp;config[taskId]=1</v>
       </c>
-      <c r="H10" s="4"/>
-      <c r="I10" s="4"/>
-    </row>
-    <row r="11" spans="1:10">
-      <c r="A11" s="4" t="s">
+      <c r="H10" s="3">
+        <v>41506</v>
+      </c>
+      <c r="I10" s="3">
+        <v>41507</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="D11" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4" t="str">
+      <c r="F11" s="6" t="str">
         <f t="shared" si="0"/>
         <v>http://wlux.uw.edu/rbwatson/task.php?config[sessionId]=1377058693&amp;config[taskId]=1</v>
       </c>
-      <c r="G11" s="4" t="str">
+      <c r="G11" s="6" t="str">
         <f t="shared" si="1"/>
         <v>http://localhost/rbwatson/task.php?config[sessionId]=1377058693&amp;config[taskId]=1</v>
       </c>
-      <c r="H11" s="4"/>
-      <c r="I11" s="4"/>
-    </row>
-    <row r="12" spans="1:10">
+      <c r="H11" s="3">
+        <v>41506</v>
+      </c>
+      <c r="I11" s="3">
+        <v>41507</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>26</v>
       </c>
@@ -966,7 +967,7 @@
       <c r="H12" s="4"/>
       <c r="I12" s="4"/>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>26</v>
       </c>
@@ -989,7 +990,7 @@
       <c r="H13" s="4"/>
       <c r="I13" s="4"/>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>26</v>
       </c>
@@ -1012,7 +1013,7 @@
       <c r="H14" s="4"/>
       <c r="I14" s="4"/>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>26</v>
       </c>
@@ -1035,7 +1036,7 @@
       <c r="H15" s="4"/>
       <c r="I15" s="4"/>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>26</v>
       </c>
@@ -1060,7 +1061,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -1075,7 +1076,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -1092,7 +1093,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>

</xml_diff>